<commit_message>
added vacations days counter
</commit_message>
<xml_diff>
--- a/2021 Mataró.xlsx
+++ b/2021 Mataró.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\Control-Horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C639AD-9FDB-489F-B025-C1487F573FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0142E6B3-883F-48C6-9B59-62B3413D4B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>January 2021</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>2021 Calendar</t>
+  </si>
+  <si>
+    <t>Días de Vacaciones</t>
   </si>
 </sst>
 </file>
@@ -2683,7 +2686,7 @@
   <dimension ref="B1:AC40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,6 +3998,9 @@
       <c r="X28" s="29">
         <v>44464</v>
       </c>
+      <c r="AA28" s="84" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B29" s="37">
@@ -4048,6 +4054,9 @@
       </c>
       <c r="W29" s="34"/>
       <c r="X29" s="36"/>
+      <c r="AA29">
+        <v>31</v>
+      </c>
     </row>
     <row r="30" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="73">

</xml_diff>